<commit_message>
Fix Product Paging API
</commit_message>
<xml_diff>
--- a/BE/DreamyShop.Infrastructure/Resources/Reports/InputReport.xlsx
+++ b/BE/DreamyShop.Infrastructure/Resources/Reports/InputReport.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1941E472-933C-4D82-A11C-F26DAB294AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980" xr2:uid="{96EF6C9B-554E-497B-8438-3D451C5B20D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -84,15 +83,9 @@
     <t>Black</t>
   </si>
   <si>
-    <t>LT-A</t>
-  </si>
-  <si>
     <t>White</t>
   </si>
   <si>
-    <t>LT-B</t>
-  </si>
-  <si>
     <t>Rolex watch</t>
   </si>
   <si>
@@ -123,27 +116,45 @@
     <t>Option Value</t>
   </si>
   <si>
-    <t>Black, 15.6</t>
-  </si>
-  <si>
     <t>White, 14</t>
   </si>
   <si>
     <t>Size</t>
   </si>
   <si>
-    <t>15.6, 14</t>
+    <t>Black, 14</t>
+  </si>
+  <si>
+    <t>LT-A2</t>
+  </si>
+  <si>
+    <t>LT-A1</t>
+  </si>
+  <si>
+    <t>LT-B1</t>
+  </si>
+  <si>
+    <t>LT-B2</t>
+  </si>
+  <si>
+    <t>15, 14</t>
+  </si>
+  <si>
+    <t>Black, 15</t>
+  </si>
+  <si>
+    <t>White, 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -155,6 +166,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -194,21 +210,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -262,7 +263,20 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -276,17 +290,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -295,45 +311,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -649,225 +686,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC148D8-930C-4715-9A81-E51CF2456B75}">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="16.75" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="5">
+        <v>22</v>
+      </c>
+      <c r="N2" s="5">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="14">
+        <v>32</v>
+      </c>
+      <c r="N3" s="14">
+        <v>4234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>11</v>
+      <c r="J4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="5">
+        <v>21</v>
+      </c>
+      <c r="N4" s="5">
+        <v>2342</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="2">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="N5" s="2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G6" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="8" t="b">
+      <c r="H6" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="I6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="3">
-        <v>22</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="L7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="3">
-        <v>15</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="b">
+      <c r="M7" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="13">
-        <v>1</v>
-      </c>
-      <c r="N4" s="13">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="N7" s="1">
         <v>11999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="22">
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="J4:J5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>